<commit_message>
Started work on the FINAL report
</commit_message>
<xml_diff>
--- a/Reports/Document List.xlsx
+++ b/Reports/Document List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/55f88cf3fb9058ce/Documents/Semester 5/Electronic Design Realization/Design Files/Reports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ACA Folder\5th Semester\EN Jaks\CEM_Design_Files\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{01976230-6CC7-40E5-9F0D-DD7A94E0A2C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{09E09139-2313-43A7-9ABB-069EEB45AF22}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0EB3859-021A-4BDE-BA1F-3DC70FE5345A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6825" xr2:uid="{5C81623E-CE56-4DCD-B1B0-DE773967F7F5}"/>
+    <workbookView xWindow="18576" yWindow="780" windowWidth="8712" windowHeight="9120" xr2:uid="{5C81623E-CE56-4DCD-B1B0-DE773967F7F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
   <si>
     <t>Document Components Needed</t>
   </si>
@@ -167,7 +167,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,6 +177,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -193,10 +199,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,27 +520,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35581FC7-41BC-4CDA-8473-4166A239D44B}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="31.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.44140625" customWidth="1"/>
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -562,7 +570,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -576,8 +584,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C4" t="s">
@@ -590,7 +598,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>25</v>
       </c>
@@ -604,7 +612,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -618,7 +626,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -632,7 +640,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -643,7 +651,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -651,7 +659,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>35</v>
       </c>
@@ -663,7 +671,7 @@
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -678,19 +686,22 @@
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
       </c>
       <c r="E12" t="s">
         <v>24</v>
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>9</v>
       </c>
@@ -705,7 +716,7 @@
       </c>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -720,7 +731,7 @@
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>11</v>
       </c>
@@ -732,7 +743,7 @@
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>16</v>
       </c>
@@ -745,7 +756,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>12</v>
       </c>
@@ -757,7 +768,7 @@
       </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>13</v>
       </c>
@@ -769,7 +780,7 @@
       </c>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>14</v>
       </c>
@@ -786,7 +797,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Design Document upto Detail design of Sensor
</commit_message>
<xml_diff>
--- a/Reports/Document List.xlsx
+++ b/Reports/Document List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ACA Folder\5th Semester\EN Jaks\CEM_Design_Files\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0EB3859-021A-4BDE-BA1F-3DC70FE5345A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5AB697-FA7D-4D14-B59C-F51B7D19AF95}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18576" yWindow="780" windowWidth="8712" windowHeight="9120" xr2:uid="{5C81623E-CE56-4DCD-B1B0-DE773967F7F5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5C81623E-CE56-4DCD-B1B0-DE773967F7F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -150,7 +150,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,8 +166,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,6 +193,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -199,11 +224,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,8 +548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35581FC7-41BC-4CDA-8473-4166A239D44B}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -580,7 +608,7 @@
       <c r="D3" t="s">
         <v>28</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -594,7 +622,7 @@
       <c r="D4" t="s">
         <v>29</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -608,7 +636,7 @@
       <c r="D5" t="s">
         <v>30</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -622,7 +650,7 @@
       <c r="D6" t="s">
         <v>29</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -636,7 +664,7 @@
       <c r="D7" t="s">
         <v>29</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -647,7 +675,7 @@
       <c r="C8" t="s">
         <v>24</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="5" t="s">
         <v>24</v>
       </c>
     </row>
@@ -669,7 +697,7 @@
       <c r="E10" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
@@ -684,7 +712,7 @@
       <c r="E11" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="2"/>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
@@ -699,7 +727,7 @@
       <c r="E12" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="2"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
@@ -714,7 +742,8 @@
       <c r="E13" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="6"/>
+      <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
@@ -729,7 +758,7 @@
       <c r="E14" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
@@ -779,6 +808,7 @@
         <v>24</v>
       </c>
       <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" t="s">

</xml_diff>